<commit_message>
Revert "Revert "multiprogram runnable""
This reverts commit ab68be797dc8991ec25a0e833db895fb3dfdce8f.
</commit_message>
<xml_diff>
--- a/examples/multiprogram/data.xlsx
+++ b/examples/multiprogram/data.xlsx
@@ -1,101 +1,163 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TvT\Desktop\RPA Examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6C812E-6FB1-43AA-BFB5-05A908702632}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22425" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Google Search Term</t>
   </si>
   <si>
+    <t>Link 1</t>
+  </si>
+  <si>
+    <t>Link 2</t>
+  </si>
+  <si>
+    <t>Link 3</t>
+  </si>
+  <si>
+    <t>Link 4</t>
+  </si>
+  <si>
+    <t>Link 5</t>
+  </si>
+  <si>
+    <t>Link 6</t>
+  </si>
+  <si>
+    <t>Link 7</t>
+  </si>
+  <si>
+    <t>Link 8</t>
+  </si>
+  <si>
+    <t>Link 9</t>
+  </si>
+  <si>
     <t>Robot</t>
   </si>
   <si>
+    <t>https://en.wikipedia.org</t>
+  </si>
+  <si>
+    <t>https://www.robots.nu</t>
+  </si>
+  <si>
+    <t>https://www.therobotreport.com</t>
+  </si>
+  <si>
+    <t>https://www.designboom.com</t>
+  </si>
+  <si>
+    <t>https://www.wired.com</t>
+  </si>
+  <si>
+    <t>https://www.livescience.com</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org</t>
+  </si>
+  <si>
+    <t>https://robots.ieee.org</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com</t>
+  </si>
+  <si>
     <t>President</t>
   </si>
   <si>
+    <t>https://www.whitehouse.gov</t>
+  </si>
+  <si>
+    <t>https://tw.dictionary.yahoo.com</t>
+  </si>
+  <si>
+    <t>https://www.merriam-webster.com</t>
+  </si>
+  <si>
+    <t>https://www.president.lv</t>
+  </si>
+  <si>
+    <t>https://president.gr</t>
+  </si>
+  <si>
+    <t>https://www.usa.gov</t>
+  </si>
+  <si>
     <t>Banana</t>
   </si>
   <si>
-    <t>Link 1</t>
-  </si>
-  <si>
-    <t>Link 2</t>
-  </si>
-  <si>
-    <t>Link 3</t>
-  </si>
-  <si>
-    <t>Link 4</t>
-  </si>
-  <si>
-    <t>Link 5</t>
-  </si>
-  <si>
-    <t>Link 6</t>
-  </si>
-  <si>
-    <t>Link 7</t>
-  </si>
-  <si>
-    <t>Link 8</t>
-  </si>
-  <si>
-    <t>Link 9</t>
+    <t>https://bananarepublic.gap.com</t>
+  </si>
+  <si>
+    <t>https://www.bananarepublic.ca</t>
+  </si>
+  <si>
+    <t>https://www.urbandictionary.com</t>
+  </si>
+  <si>
+    <t>https://bananarepublicfactory.gapfactory.com</t>
+  </si>
+  <si>
+    <t>https://www.bananarepublicfactory.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="等线"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,32 +201,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -459,81 +512,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="150" zoomScaleNormal="150">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="23.625"/>
+    <col customWidth="1" max="2" min="2" width="32.875"/>
+    <col customWidth="1" max="3" min="3" width="38.375"/>
+    <col customWidth="1" max="4" min="4" width="33.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="1" spans="1:10" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row customHeight="1" ht="15" r="2" spans="1:10" thickBot="1">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="3" spans="1:10" thickBot="1">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="4" spans="1:10" thickBot="1">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="5" spans="1:10" thickBot="1">
+      <c r="A5" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="6" spans="1:10" thickBot="1">
+      <c r="A6" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="7" spans="1:10" thickBot="1">
+      <c r="A7" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="8" spans="1:10" thickBot="1">
+      <c r="A8" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="9" spans="1:10" thickBot="1">
+      <c r="A9" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="10" spans="1:10" thickBot="1">
+      <c r="A10" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>